<commit_message>
Need to rework the symbol library
</commit_message>
<xml_diff>
--- a/Card/L1IFStream_BOM.xlsx
+++ b/Card/L1IFStream_BOM.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\GPS\L1IFStream\Card\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{053DF159-1CFD-44CF-B0D6-76D3967364C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8A95D5-132E-4A29-B103-766E81DF4896}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="3790" windowWidth="25020" windowHeight="16970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="820" yWindow="3200" windowWidth="25020" windowHeight="16970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="L1IFStream" sheetId="1" r:id="rId1"/>
@@ -1540,7 +1540,7 @@
   <dimension ref="A1:J51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>